<commit_message>
adding the same tables of Cumulative Analysis (CA) for Indiana Vs National
</commit_message>
<xml_diff>
--- a/ATC/exported_analysis/ATC2_CA_comparing.xlsx
+++ b/ATC/exported_analysis/ATC2_CA_comparing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/lholguin_purdue_edu/Documents/VS code/Data/ATC/exported_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{EAC35ADF-3472-43AE-B415-8D2D1FAB817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75D75B46-65A1-40A0-8D59-2E68013058FE}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{EAC35ADF-3472-43AE-B415-8D2D1FAB817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8F9A66-8FA0-4FDA-880C-D4E5A0D449B2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="5060" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units_Reimbursed" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="128">
   <si>
     <t>ATC_Class</t>
   </si>
@@ -413,12 +413,21 @@
   <si>
     <t>VLOOKUP GENERAL</t>
   </si>
+  <si>
+    <t>Indiana Vs NATIONAL (ANALYSIS - ACROSS)</t>
+  </si>
+  <si>
+    <t>Comparing units Vs prescriptions in Indiana state</t>
+  </si>
+  <si>
+    <t>Comparing units Vs prescriptions NATIONALLY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +444,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -525,6 +542,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,6 +566,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -829,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection sqref="A1:M87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4415,7 +4445,7 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection sqref="A1:M87"/>
+      <selection activeCell="J2" sqref="J2:J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7996,7 +8026,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C8D169-525D-4333-962A-DB250C299FA0}">
   <dimension ref="A1:AE87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8195,7 +8227,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B66" si="0">VLOOKUP(A3,$R$2:$R$29,1,0)</f>
+        <f t="shared" ref="B3:B23" si="0">VLOOKUP(A3,$R$2:$R$29,1,0)</f>
         <v>N02</v>
       </c>
       <c r="C3">
@@ -15191,11 +15223,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70ED9936-71FC-4775-B375-96890ACDBCDF}">
   <dimension ref="B2:AH61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="18" max="18" width="18.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:34" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -15206,9 +15241,27 @@
       <c r="B4" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="U4" s="6" t="s">
         <v>123</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+    </row>
+    <row r="5" spans="2:34" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.35">
@@ -20031,6 +20084,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="W4:AA4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>